<commit_message>
PID to PD switch
</commit_message>
<xml_diff>
--- a/condition_file.xlsx
+++ b/condition_file.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -399,7 +399,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -413,29 +413,53 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>

</xml_diff>